<commit_message>
feat(phone): add stylesheet 720x1280
</commit_message>
<xml_diff>
--- a/docs/_static/tools/stylesheet_calculator.xlsx
+++ b/docs/_static/tools/stylesheet_calculator.xlsx
@@ -714,7 +714,7 @@
   <dimension ref="C4:O29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -955,7 +955,7 @@
         <v>60</v>
       </c>
       <c r="O13" s="7" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +979,7 @@
         <v>22</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="O15" s="2" t="n">
         <f aca="false">O16 / O5 * O4</f>
-        <v>567</v>
+        <v>555.75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="O16" s="2" t="n">
         <f aca="false">O11 - O13</f>
-        <v>1008</v>
+        <v>988</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="O22" s="29" t="n">
         <f aca="false">O19 + O13</f>
-        <v>860</v>
+        <v>880</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>